<commit_message>
redaccion req anal v1
</commit_message>
<xml_diff>
--- a/Plantilla-Hoja Temas analíticos - Copy.xlsx
+++ b/Plantilla-Hoja Temas analíticos - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orjue\Desktop\BI\parcial2\proyecto-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F977085-F480-4983-869F-9178A0EB304D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A042254A-23DD-4C87-9632-FCF9307A6D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1335" windowWidth="16785" windowHeight="9570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temas Analíticos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="30">
   <si>
     <t>Formato para documentar los temas analíticos y análisis requeridos identificados a partir de las entrevistas</t>
   </si>
@@ -40,15 +40,9 @@
     <t>Fuentes de datos y datos</t>
   </si>
   <si>
-    <t xml:space="preserve">Comportamiento de la población demográfica por indicador </t>
-  </si>
-  <si>
     <t>Tablero de control</t>
   </si>
   <si>
-    <t>Cobertura de la educación en Colombia</t>
-  </si>
-  <si>
     <t>Extracción de tasa de analfabetismo por departamento por año y por nivel de urbanización (urbano o rural)</t>
   </si>
   <si>
@@ -64,7 +58,58 @@
     <t>Extracción del indicador de cobertura neta total por departamento y año</t>
   </si>
   <si>
-    <t>Visualización de la tasa de analfabetismo cruzado con la cobeertura neta total en la educación utilizando un mapa de Colombia</t>
+    <t>Extracción del porcentaje de hombres y mujeres por departamento por año</t>
+  </si>
+  <si>
+    <t>TerriData - Demografia Y Poblacion.xslx</t>
+  </si>
+  <si>
+    <t>Tasas de analfabetismo y cobertura de educación en Colombia</t>
+  </si>
+  <si>
+    <t>Visualización del porcentaje de hombres y mujeres por año utilizando un mapa de Colombia</t>
+  </si>
+  <si>
+    <t>Extracción de la cantidad de población rural y urbana por departamento por año</t>
+  </si>
+  <si>
+    <t>Visualización de la cantidad de población rural y urbana utilizando un mapa de Colombia</t>
+  </si>
+  <si>
+    <t>Comportamiento de la población demográfica por género y nivel de urbanización en Colombia</t>
+  </si>
+  <si>
+    <t>Tasas de deserción intra-anual y repitencia del sector oficial en educación básica y media en Colombia</t>
+  </si>
+  <si>
+    <t>Visualización de la tasa de deserción intra-anual cruzado con la tasa de repitencia utilizando un mapa de Colombia</t>
+  </si>
+  <si>
+    <t>Visualización de la tasa de analfabetismo cruzado con la cobertura neta total en la educación utilizando un mapa de Colombia</t>
+  </si>
+  <si>
+    <t>Extracción de la tasa de deserción intra-anual por departamento por año</t>
+  </si>
+  <si>
+    <t>Extracción de la tasa de repitencia por departamento por año</t>
+  </si>
+  <si>
+    <t>TerriData - Salud.xslx</t>
+  </si>
+  <si>
+    <t>TerriData - Vivienda y Servicios Publicos.xslx</t>
+  </si>
+  <si>
+    <t>Cobertura de alcantarillado y acueducto en Colombia</t>
+  </si>
+  <si>
+    <t>Extracción de la cobertura de alcantarillado por departamento por año</t>
+  </si>
+  <si>
+    <t>Extracción de la cobertura de acueducto por departamento por año</t>
+  </si>
+  <si>
+    <t>Visualización de la cobertura de alcantarillado cruzado con la cobertura de acueducto utilizando un mapa de Colombia</t>
   </si>
 </sst>
 </file>
@@ -102,7 +147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -302,19 +347,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -336,36 +368,16 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -380,31 +392,16 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -413,6 +410,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -431,28 +440,28 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -793,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A5:E62"/>
+  <dimension ref="A5:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:E20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,432 +824,546 @@
     </row>
     <row r="8" spans="1:5" ht="0.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:5" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+    <row r="10" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-    </row>
-    <row r="15" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
-    </row>
-    <row r="16" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="D12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22"/>
+      <c r="B13" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="26"/>
+    </row>
+    <row r="15" spans="1:5" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="D16" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="E16" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="27" t="s">
+    </row>
+    <row r="17" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="32"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="26"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="34"/>
-    </row>
-    <row r="21" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="15"/>
-    </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17"/>
-    </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="13"/>
-    </row>
-    <row r="27" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
+    </row>
+    <row r="18" spans="1:5" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="22"/>
+      <c r="B18" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="30"/>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="18"/>
+      <c r="B23" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="27"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="29"/>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="9"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="23"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="13"/>
-    </row>
-    <row r="33" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="19"/>
-    </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="7"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="19"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="27"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="29"/>
+    </row>
+    <row r="31" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="18"/>
+      <c r="B34" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="11"/>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="7"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="9"/>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="23"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="13"/>
-    </row>
-    <row r="39" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="19"/>
-    </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="7"/>
-    </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="7"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="18"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="18"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="19"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="11"/>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="7"/>
+      <c r="A42" s="17"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="9"/>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="23"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="13"/>
-    </row>
-    <row r="45" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="5"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="19"/>
-    </row>
-    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="7"/>
-    </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="7"/>
+      <c r="A43" s="18"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="19"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="11"/>
     </row>
     <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="7"/>
+      <c r="A48" s="17"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="4"/>
     </row>
     <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="9"/>
-    </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="23"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="13"/>
-    </row>
-    <row r="51" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="5"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="19"/>
-    </row>
-    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="7"/>
-    </row>
-    <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="7"/>
+      <c r="A49" s="18"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="19"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="8"/>
+    </row>
+    <row r="53" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="11"/>
     </row>
     <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="22"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="7"/>
+      <c r="A54" s="17"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="4"/>
     </row>
     <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="22"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="9"/>
-    </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="23"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="13"/>
-    </row>
-    <row r="57" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="5"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="19"/>
-    </row>
-    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="21"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="7"/>
-    </row>
-    <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="22"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="7"/>
-    </row>
-    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="7"/>
-    </row>
-    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="22"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="9"/>
-    </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="23"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="13"/>
+      <c r="A55" s="18"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="18"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="18"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="6"/>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="19"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A58:A62"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A34:A38"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A32:A34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1248,18 +1371,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1453,18 +1576,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A078967-5430-4F36-AE44-54F6FF19905C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF57A317-E2FD-461A-8FCD-E863AC62598A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF57A317-E2FD-461A-8FCD-E863AC62598A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A078967-5430-4F36-AE44-54F6FF19905C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update Plantilla-Hoja Temas analíticos - Copy.xlsx
</commit_message>
<xml_diff>
--- a/Plantilla-Hoja Temas analíticos - Copy.xlsx
+++ b/Plantilla-Hoja Temas analíticos - Copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orjue\Desktop\BI\parcial2\proyecto-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rembrandtsx/Documents/repos/GitHub/proyecto-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A042254A-23DD-4C87-9632-FCF9307A6D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0671D8-5F13-8145-A92D-F9F02811571A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24580" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temas Analíticos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="41">
   <si>
     <t>Formato para documentar los temas analíticos y análisis requeridos identificados a partir de las entrevistas</t>
   </si>
@@ -110,6 +110,39 @@
   </si>
   <si>
     <t>Visualización de la cobertura de alcantarillado cruzado con la cobertura de acueducto utilizando un mapa de Colombia</t>
+  </si>
+  <si>
+    <t>Correlación entre cobertura de vacunacion (DPT, Triple Viral, y pentavalente menores de 1 año) con el registro especial de prestadores y sedes de servicios de salud en Colombia</t>
+  </si>
+  <si>
+    <t>Extracción y geolocalizacion de los prestadores y sedes de servicios de salud.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extracción tasa de vacunación (DPT,Tripe Viral, y Pentavalente) por departamento </t>
+  </si>
+  <si>
+    <t>Visualización de las tasas por departamento de vacunación (DPT, Triple Viral y Pentavalente) en el mapa colombiano</t>
+  </si>
+  <si>
+    <t>Visualización de los centros de salud en el mapa colombiano</t>
+  </si>
+  <si>
+    <t>Visualización del cruzado de tasas de vacunación por departamento vs cantidad de sedes de servicios de salud en Colombia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encuesta interna de datos Ministerio de Salud y Protección Social - Dirección de Prestación de Servicios y Atención Primaria </t>
+  </si>
+  <si>
+    <t>Tabulación datos vacunación nacionales por parte del Ministerio de Salud y Protección Social</t>
+  </si>
+  <si>
+    <t>Encuesta interna de datos Ministerio de Salud y Protección Social - Dirección de Prestación de Servicios y Atención Primaria /  Tabulación datos vacunación nacionales por parte del Ministerio de Salud y Protección Social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TerriData - Salud.xslx y datos.gov.co ( https://www.datos.gov.co/Salud-y-Protecci-n-Social/Registro-Especial-de-Prestadores-y-Sedes-de-Servic/c36g-9fc2/ ) datos locales en: datos/Registro_Especial_de_Prestadores_y_Sedes_de_Servicios_de_Salud.csv </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> datos.gov.co ( https://www.datos.gov.co/Salud-y-Protecci-n-Social/Registro-Especial-de-Prestadores-y-Sedes-de-Servic/c36g-9fc2/ ) datos locales en: datos/Registro_Especial_de_Prestadores_y_Sedes_de_Servicios_de_Salud.csv </t>
   </si>
 </sst>
 </file>
@@ -422,6 +455,30 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -438,30 +495,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -482,7 +515,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -802,28 +835,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A5:E58"/>
+  <dimension ref="A5:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="117" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" style="1" customWidth="1"/>
-    <col min="2" max="3" width="41.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="2" max="3" width="41.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="0.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:5" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:5" ht="0.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:5" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>1</v>
       </c>
@@ -836,12 +870,12 @@
       <c r="D9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -857,8 +891,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+    <row r="11" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="29"/>
       <c r="B11" s="14" t="s">
         <v>16</v>
       </c>
@@ -872,8 +906,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+    <row r="12" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="29"/>
       <c r="B12" s="15" t="s">
         <v>15</v>
       </c>
@@ -887,8 +921,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
+    <row r="13" spans="1:5" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
       <c r="B13" s="16" t="s">
         <v>17</v>
       </c>
@@ -902,14 +936,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="26"/>
-    </row>
-    <row r="15" spans="1:5" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
+    </row>
+    <row r="15" spans="1:5" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>1</v>
       </c>
@@ -926,8 +960,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+    <row r="16" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="28" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="14" t="s">
@@ -943,8 +977,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+    <row r="17" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="29"/>
       <c r="B17" s="14" t="s">
         <v>11</v>
       </c>
@@ -958,8 +992,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
+    <row r="18" spans="1:5" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="30"/>
       <c r="B18" s="16" t="s">
         <v>21</v>
       </c>
@@ -973,14 +1007,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="30"/>
-    </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="24"/>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
@@ -997,8 +1031,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+    <row r="21" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="25" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="13" t="s">
@@ -1014,8 +1048,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
+    <row r="22" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="26"/>
       <c r="B22" s="13" t="s">
         <v>23</v>
       </c>
@@ -1029,8 +1063,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="18"/>
+    <row r="23" spans="1:5" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
       <c r="B23" s="14" t="s">
         <v>20</v>
       </c>
@@ -1044,14 +1078,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="29"/>
-    </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="23"/>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>1</v>
       </c>
@@ -1068,97 +1102,113 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
+    <row r="26" spans="1:5" ht="142" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="D26" s="14" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="26"/>
+      <c r="B27" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="D27" s="14" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
+    <row r="28" spans="1:5" ht="145" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="26"/>
+      <c r="B28" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>6</v>
+      </c>
       <c r="D28" s="14" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="19"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16" t="s">
-        <v>9</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="26"/>
+      <c r="B29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="140" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="29"/>
-    </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
+      <c r="B30" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="21"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="23"/>
+    </row>
+    <row r="32" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B32" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C32" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D32" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E32" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+    <row r="33" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B33" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="13" t="s">
-        <v>28</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>8</v>
@@ -1170,13 +1220,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="18"/>
-      <c r="B34" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>6</v>
+    <row r="34" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="26"/>
+      <c r="B34" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>8</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>9</v>
@@ -1185,185 +1235,200 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="11"/>
-    </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
+    <row r="35" spans="1:5" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="26"/>
+      <c r="B35" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="11"/>
+    </row>
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="25"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="26"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="6"/>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="19"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="11"/>
-    </row>
-    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="26"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="26"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="27"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="8"/>
+    </row>
+    <row r="42" spans="1:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="11"/>
+    </row>
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="25"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
       <c r="E43" s="4"/>
     </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="26"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="4"/>
     </row>
-    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="6"/>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="19"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="8"/>
-    </row>
-    <row r="47" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="11"/>
-    </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="4"/>
-    </row>
-    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
+    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="26"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="26"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="27"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" spans="1:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="11"/>
+    </row>
+    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="25"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
       <c r="E49" s="4"/>
     </row>
-    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
+    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="26"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="4"/>
     </row>
-    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="18"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="6"/>
-    </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="19"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="8"/>
-    </row>
-    <row r="53" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="11"/>
-    </row>
-    <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="4"/>
-    </row>
-    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="18"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="26"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="26"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="6"/>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="27"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="8"/>
+    </row>
+    <row r="54" spans="1:5" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="11"/>
+    </row>
+    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="25"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
       <c r="E55" s="4"/>
     </row>
-    <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="18"/>
+    <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="26"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="4"/>
     </row>
-    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="18"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="6"/>
-    </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="19"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="8"/>
+    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="26"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="26"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="6"/>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="27"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="A55:A59"/>
     <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="A49:A53"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="A33:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1371,21 +1436,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F7B2620488C365419ACDBBCCE69988B8" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="18b322838a1aba3a124f28c6eda8158c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8efacf54-3af5-4846-9aca-6e8169fe1a0e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9806dd69421cff2fc866557e390a69b9" ns2:_="">
     <xsd:import namespace="8efacf54-3af5-4846-9aca-6e8169fe1a0e"/>
@@ -1575,24 +1625,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF57A317-E2FD-461A-8FCD-E863AC62598A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A078967-5430-4F36-AE44-54F6FF19905C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB9F01E6-3AC0-45F6-920B-DBC80B5A0281}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1608,4 +1656,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A078967-5430-4F36-AE44-54F6FF19905C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF57A317-E2FD-461A-8FCD-E863AC62598A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>